<commit_message>
18/10/24; official goalscorer ranking
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedrohamacher\OneDrive\Documentos antigo\Projetos_jl\Streamlit\Dashboard Pelada\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="97" documentId="14_{C36D493D-CB08-48D2-969C-03F43E1F90CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{D8132BC9-A131-44AA-943A-16E1DA8C9916}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="113_{0AE4E784-A55A-46D6-B24A-1982B84D5895}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{BEFC8A70-B090-4F6E-ADC6-3D6AAB34A326}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="3780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="3780" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="notas" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="66">
   <si>
     <t>Jogador</t>
   </si>
@@ -219,7 +219,10 @@
     <t>Queiroga</t>
   </si>
   <si>
-    <t>Gols</t>
+    <t>Gols oficiais</t>
+  </si>
+  <si>
+    <t>Gols (total)</t>
   </si>
 </sst>
 </file>
@@ -1216,9 +1219,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF42"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="T39" sqref="T39"/>
+      <selection pane="topRight" activeCell="W13" sqref="W13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1233,6 +1236,7 @@
     <col min="16" max="18" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.3">
@@ -1296,6 +1300,9 @@
       <c r="T1" s="1">
         <v>45574</v>
       </c>
+      <c r="U1" s="1">
+        <v>45581</v>
+      </c>
       <c r="AC1" t="s">
         <v>57</v>
       </c>
@@ -1370,17 +1377,20 @@
       <c r="T2">
         <v>6</v>
       </c>
+      <c r="U2">
+        <v>5.5</v>
+      </c>
       <c r="AC2">
         <f t="shared" ref="AC2:AC42" si="0">COUNT(B2:AB2)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="AD2" s="18">
         <f t="shared" ref="AD2:AD42" si="1">AVERAGE(B2:AB2)</f>
-        <v>6.2368421052631575</v>
+        <v>6.2</v>
       </c>
       <c r="AE2">
         <f t="shared" ref="AE2:AE42" si="2">IF(AC2&gt;1,_xlfn.STDEV.S(B2:AB2),"")</f>
-        <v>0.80568157917228478</v>
+        <v>0.80131470918603331</v>
       </c>
       <c r="AF2">
         <v>1</v>
@@ -1447,17 +1457,20 @@
       <c r="T3">
         <v>5.5</v>
       </c>
+      <c r="U3">
+        <v>6.5</v>
+      </c>
       <c r="AC3">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="AD3" s="18">
         <f t="shared" si="1"/>
-        <v>5.7631578947368425</v>
+        <v>5.8</v>
       </c>
       <c r="AE3">
         <f t="shared" si="2"/>
-        <v>0.56195148694901631</v>
+        <v>0.57124057057747935</v>
       </c>
       <c r="AF3">
         <v>1</v>
@@ -1521,17 +1534,20 @@
       <c r="T4">
         <v>7</v>
       </c>
+      <c r="U4">
+        <v>6.5</v>
+      </c>
       <c r="AC4">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="AD4" s="18">
         <f t="shared" si="1"/>
-        <v>6.5555555555555554</v>
+        <v>6.5526315789473681</v>
       </c>
       <c r="AE4">
         <f t="shared" si="2"/>
-        <v>0.48169092143287223</v>
+        <v>0.46829290579084676</v>
       </c>
       <c r="AF4">
         <v>1</v>
@@ -1592,17 +1608,20 @@
       <c r="T5">
         <v>6.5</v>
       </c>
+      <c r="U5">
+        <v>6</v>
+      </c>
       <c r="AC5">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AD5" s="18">
         <f t="shared" si="1"/>
-        <v>5.9411764705882355</v>
+        <v>5.9444444444444446</v>
       </c>
       <c r="AE5">
         <f t="shared" si="2"/>
-        <v>0.46376020680063168</v>
+        <v>0.45012706993133311</v>
       </c>
       <c r="AF5">
         <v>1</v>
@@ -1660,17 +1679,20 @@
       <c r="T6">
         <v>6</v>
       </c>
+      <c r="U6">
+        <v>6.5</v>
+      </c>
       <c r="AC6">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AD6" s="18">
         <f t="shared" si="1"/>
-        <v>6.25</v>
+        <v>6.2647058823529411</v>
       </c>
       <c r="AE6">
         <f t="shared" si="2"/>
-        <v>0.54772255750516607</v>
+        <v>0.53378504155533923</v>
       </c>
       <c r="AF6">
         <v>1</v>
@@ -1728,17 +1750,20 @@
       <c r="T7">
         <v>5.5</v>
       </c>
+      <c r="U7">
+        <v>5.5</v>
+      </c>
       <c r="AC7">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AD7" s="18">
         <f t="shared" si="1"/>
-        <v>5.75</v>
+        <v>5.7352941176470589</v>
       </c>
       <c r="AE7">
         <f t="shared" si="2"/>
-        <v>0.5163977794943222</v>
+        <v>0.50366305263363853</v>
       </c>
       <c r="AF7">
         <v>1</v>
@@ -1793,17 +1818,20 @@
       <c r="Q8">
         <v>6.5</v>
       </c>
+      <c r="U8">
+        <v>6.5</v>
+      </c>
       <c r="AC8">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AD8" s="18">
         <f t="shared" si="1"/>
-        <v>7.0666666666666664</v>
+        <v>7.03125</v>
       </c>
       <c r="AE8">
         <f t="shared" si="2"/>
-        <v>0.56273143387113755</v>
+        <v>0.5618051263561058</v>
       </c>
       <c r="AF8">
         <v>1</v>
@@ -1858,17 +1886,20 @@
       <c r="T9">
         <v>6.5</v>
       </c>
+      <c r="U9">
+        <v>6</v>
+      </c>
       <c r="AC9">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AD9" s="18">
         <f t="shared" si="1"/>
-        <v>6.5333333333333332</v>
+        <v>6.5</v>
       </c>
       <c r="AE9">
         <f t="shared" si="2"/>
-        <v>0.71879528842826157</v>
+        <v>0.70710678118654757</v>
       </c>
       <c r="AF9">
         <v>1</v>
@@ -2047,17 +2078,20 @@
       <c r="T12">
         <v>6.5</v>
       </c>
+      <c r="U12">
+        <v>6.5</v>
+      </c>
       <c r="AC12">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="AD12" s="18">
         <f t="shared" si="1"/>
-        <v>6.4615384615384617</v>
+        <v>6.4642857142857144</v>
       </c>
       <c r="AE12">
         <f t="shared" si="2"/>
-        <v>0.43115824925128815</v>
+        <v>0.41437096508237242</v>
       </c>
       <c r="AF12">
         <v>1</v>
@@ -2274,17 +2308,20 @@
       <c r="T16">
         <v>6</v>
       </c>
+      <c r="U16">
+        <v>3.5</v>
+      </c>
       <c r="AC16">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="AD16" s="18">
         <f t="shared" si="1"/>
-        <v>5.0909090909090908</v>
+        <v>4.958333333333333</v>
       </c>
       <c r="AE16">
         <f t="shared" si="2"/>
-        <v>0.76870611478580908</v>
+        <v>0.86493124617281714</v>
       </c>
       <c r="AF16">
         <v>1</v>
@@ -2374,17 +2411,20 @@
       <c r="T18">
         <v>6</v>
       </c>
+      <c r="U18">
+        <v>6</v>
+      </c>
       <c r="AC18">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AD18" s="18">
         <f t="shared" si="1"/>
-        <v>6.4</v>
+        <v>6.3636363636363633</v>
       </c>
       <c r="AE18">
         <f t="shared" si="2"/>
-        <v>0.77459666924148174</v>
+        <v>0.74467808786445178</v>
       </c>
       <c r="AF18">
         <v>1</v>
@@ -2468,17 +2508,20 @@
       <c r="T20">
         <v>6</v>
       </c>
+      <c r="U20">
+        <v>6.5</v>
+      </c>
       <c r="AC20">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AD20" s="18">
         <f t="shared" si="1"/>
-        <v>5.8888888888888893</v>
+        <v>5.95</v>
       </c>
       <c r="AE20">
         <f t="shared" si="2"/>
-        <v>0.48591265790377502</v>
+        <v>0.49721446300587657</v>
       </c>
       <c r="AF20">
         <v>1</v>
@@ -2515,9 +2558,12 @@
       <c r="Q21">
         <v>5</v>
       </c>
+      <c r="U21">
+        <v>5.5</v>
+      </c>
       <c r="AC21">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AD21" s="18">
         <f t="shared" si="1"/>
@@ -2525,7 +2571,7 @@
       </c>
       <c r="AE21">
         <f t="shared" si="2"/>
-        <v>0.8660254037844386</v>
+        <v>0.81649658092772603</v>
       </c>
       <c r="AF21">
         <v>0</v>
@@ -2559,17 +2605,20 @@
       <c r="O22">
         <v>5.5</v>
       </c>
+      <c r="U22">
+        <v>6</v>
+      </c>
       <c r="AC22">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AD22" s="18">
         <f t="shared" si="1"/>
-        <v>5.5</v>
+        <v>5.5555555555555554</v>
       </c>
       <c r="AE22">
         <f t="shared" si="2"/>
-        <v>0.80178372573727319</v>
+        <v>0.7682953714410744</v>
       </c>
       <c r="AF22">
         <v>1</v>
@@ -2702,17 +2751,20 @@
       <c r="R26">
         <v>6.5</v>
       </c>
+      <c r="U26">
+        <v>6.5</v>
+      </c>
       <c r="AC26">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AD26" s="18">
         <f t="shared" si="1"/>
-        <v>6.625</v>
+        <v>6.6</v>
       </c>
       <c r="AE26">
         <f t="shared" si="2"/>
-        <v>0.25</v>
+        <v>0.22360679774997896</v>
       </c>
       <c r="AF26">
         <v>0</v>
@@ -2731,17 +2783,20 @@
       <c r="T27">
         <v>6.5</v>
       </c>
+      <c r="U27">
+        <v>6.5</v>
+      </c>
       <c r="AC27">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AD27" s="18">
         <f t="shared" si="1"/>
-        <v>5.833333333333333</v>
+        <v>6</v>
       </c>
       <c r="AE27">
         <f t="shared" si="2"/>
-        <v>0.76376261582597493</v>
+        <v>0.70710678118654757</v>
       </c>
       <c r="AF27">
         <v>1</v>
@@ -2867,17 +2922,20 @@
       <c r="T32">
         <v>4.5</v>
       </c>
+      <c r="U32">
+        <v>4.5</v>
+      </c>
       <c r="AC32">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AD32" s="18">
         <f t="shared" si="1"/>
-        <v>4.75</v>
+        <v>4.666666666666667</v>
       </c>
       <c r="AE32">
         <f t="shared" si="2"/>
-        <v>0.35355339059327379</v>
+        <v>0.28867513459481287</v>
       </c>
       <c r="AF32">
         <v>0</v>
@@ -3106,24 +3164,39 @@
       <c r="S42">
         <v>5</v>
       </c>
+      <c r="U42">
+        <v>5</v>
+      </c>
       <c r="AC42">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD42" s="18">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="AE42" t="str">
+      <c r="AE42">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="AF42">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:AA38">
+  <conditionalFormatting sqref="B2:T38 V2:AA38">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:Q39">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
@@ -3135,8 +3208,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:Q39">
-    <cfRule type="colorScale" priority="12">
+  <conditionalFormatting sqref="AC2:AC39">
+    <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3147,7 +3220,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC2:AC39">
+  <conditionalFormatting sqref="AE2:AE39">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC40:AC42">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
@@ -3159,7 +3244,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE2:AE39">
+  <conditionalFormatting sqref="AE40:AE42">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -3171,7 +3256,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC40:AC42">
+  <conditionalFormatting sqref="B43:AA47 B2:T42 V2:AA42">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -3183,19 +3268,31 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE40:AE42">
+  <conditionalFormatting sqref="AC2:AC42">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD2:AD39">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
-        <color rgb="FF5A8AC6"/>
-        <color rgb="FFFCFCFF"/>
         <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:AA47">
+  <conditionalFormatting sqref="AD40:AD42">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -3207,7 +3304,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC2:AC42">
+  <conditionalFormatting sqref="AD2:AD42">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -3219,7 +3316,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AD2:AD39">
+  <conditionalFormatting sqref="U2:U38">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -3231,7 +3328,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AD40:AD42">
+  <conditionalFormatting sqref="U2:U42">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -3243,7 +3340,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AD2:AD42">
+  <conditionalFormatting sqref="F2:AA42">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -3261,15 +3358,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:P56"/>
+  <dimension ref="A1:P59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="I62" sqref="I62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
@@ -6058,6 +6155,156 @@
       </c>
       <c r="P56" s="8" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A57" s="14">
+        <v>45581</v>
+      </c>
+      <c r="B57" s="3">
+        <v>5</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D57" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E57" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F57" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G57" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="H57" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="I57" s="9">
+        <v>3</v>
+      </c>
+      <c r="J57" s="10">
+        <v>7</v>
+      </c>
+      <c r="K57" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="L57" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="M57" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="N57" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="O57" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="P57" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A58" s="14">
+        <v>45581</v>
+      </c>
+      <c r="B58" s="3">
+        <v>5</v>
+      </c>
+      <c r="C58" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D58" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E58" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F58" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G58" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H58" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I58" s="11">
+        <v>3</v>
+      </c>
+      <c r="J58" s="2">
+        <v>4</v>
+      </c>
+      <c r="K58" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L58" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M58" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="N58" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="O58" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="P58" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A59" s="14">
+        <v>45581</v>
+      </c>
+      <c r="B59" s="5">
+        <v>4</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H59" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I59" s="5">
+        <v>3</v>
+      </c>
+      <c r="J59" s="8">
+        <v>2</v>
+      </c>
+      <c r="K59" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="L59" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="M59" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="N59" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="O59" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="P59" s="8" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -6067,10 +6314,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40949BC3-8DAE-4185-A4C0-F8573FA5A3A2}">
-  <dimension ref="A1:AC42"/>
+  <dimension ref="A1:AD42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="AC2" sqref="AC2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6081,9 +6328,10 @@
     <col min="8" max="10" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.5546875" bestFit="1" customWidth="1"/>
     <col min="12" max="16" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6132,11 +6380,17 @@
       <c r="P1" s="1">
         <v>45574</v>
       </c>
+      <c r="Q1" s="1">
+        <v>45581</v>
+      </c>
       <c r="AC1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -6150,14 +6404,21 @@
         <v>1</v>
       </c>
       <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
         <v>1</v>
       </c>
       <c r="AC2">
         <f>SUM(B2:AB2)</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="AD2">
+        <f>SUM(Q2:AB2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -6176,12 +6437,19 @@
       <c r="K3">
         <v>3</v>
       </c>
+      <c r="Q3">
+        <v>2</v>
+      </c>
       <c r="AC3">
         <f t="shared" ref="AC3:AC42" si="0">SUM(B3:AB3)</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="AD3">
+        <f t="shared" ref="AD3:AD42" si="1">SUM(Q3:AB3)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -6200,12 +6468,19 @@
       <c r="K4">
         <v>1</v>
       </c>
+      <c r="Q4">
+        <v>2</v>
+      </c>
       <c r="AC4">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="AD4">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -6222,8 +6497,12 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -6242,12 +6521,19 @@
       <c r="I6">
         <v>1</v>
       </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
       <c r="AC6">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+      <c r="AD6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -6261,8 +6547,12 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -6275,24 +6565,38 @@
       <c r="K8">
         <v>3</v>
       </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
       <c r="AC8">
         <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="AD8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>23</v>
       </c>
       <c r="E9">
         <v>2</v>
       </c>
+      <c r="Q9">
+        <v>1</v>
+      </c>
       <c r="AC9">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="AD9">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -6312,8 +6616,12 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -6324,8 +6632,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -6338,12 +6650,19 @@
       <c r="K12">
         <v>3</v>
       </c>
+      <c r="Q12">
+        <v>3</v>
+      </c>
       <c r="AC12">
         <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+      <c r="AD12">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -6351,8 +6670,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -6363,8 +6686,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -6375,8 +6702,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -6390,8 +6721,12 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -6408,17 +6743,28 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>19</v>
       </c>
+      <c r="Q18">
+        <v>2</v>
+      </c>
       <c r="AC18">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="AD18">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>45</v>
       </c>
@@ -6438,8 +6784,12 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -6447,8 +6797,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>46</v>
       </c>
@@ -6461,24 +6815,38 @@
       <c r="K21">
         <v>4</v>
       </c>
+      <c r="Q21">
+        <v>1</v>
+      </c>
       <c r="AC21">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+      <c r="AD21">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>8</v>
       </c>
       <c r="G22">
         <v>1</v>
       </c>
+      <c r="Q22">
+        <v>1</v>
+      </c>
       <c r="AC22">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="AD22">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -6492,8 +6860,12 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -6501,8 +6873,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD24">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -6516,8 +6892,12 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>48</v>
       </c>
@@ -6525,17 +6905,28 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>55</v>
       </c>
+      <c r="Q27">
+        <v>2</v>
+      </c>
       <c r="AC27">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="AD27">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>61</v>
       </c>
@@ -6543,8 +6934,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>18</v>
       </c>
@@ -6552,8 +6947,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>56</v>
       </c>
@@ -6564,8 +6963,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>17</v>
       </c>
@@ -6573,17 +6976,28 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>60</v>
       </c>
+      <c r="Q32">
+        <v>2</v>
+      </c>
       <c r="AC32">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="AD32">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>51</v>
       </c>
@@ -6594,8 +7008,12 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>21</v>
       </c>
@@ -6603,8 +7021,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD34">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>43</v>
       </c>
@@ -6612,8 +7034,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>16</v>
       </c>
@@ -6621,8 +7047,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>52</v>
       </c>
@@ -6633,8 +7063,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD37">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>54</v>
       </c>
@@ -6642,8 +7076,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>49</v>
       </c>
@@ -6654,8 +7092,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD39">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>53</v>
       </c>
@@ -6663,8 +7105,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD40">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>47</v>
       </c>
@@ -6675,14 +7121,25 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>63</v>
       </c>
+      <c r="Q42">
+        <v>2</v>
+      </c>
       <c r="AC42">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="AD42">
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>